<commit_message>
[CP-1] Tomashevskyi (FB-31), Tkach (FB-31)
</commit_message>
<xml_diff>
--- a/lab1/tomashevskyi_fb-31_tkach_fb-31_cp1/lab1_results.xlsx
+++ b/lab1/tomashevskyi_fb-31_tkach_fb-31_cp1/lab1_results.xlsx
@@ -16409,12 +16409,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>0,60033</t>
+          <t>0,20065</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>0,58866</t>
+          <t>0,17732</t>
         </is>
       </c>
     </row>
@@ -16443,12 +16443,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>0,60044</t>
+          <t>0,20088</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>0,58881</t>
+          <t>0,17761</t>
         </is>
       </c>
     </row>

</xml_diff>